<commit_message>
Add empty sheet to test file
</commit_message>
<xml_diff>
--- a/tests/fixtures/formats/sample_headers.xlsx
+++ b/tests/fixtures/formats/sample_headers.xlsx
@@ -5,10 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -146,11 +147,11 @@
   </sheetPr>
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -192,4 +193,27 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Revert "Add empty sheet to test file"
This reverts commit a4bf38a31d7e242a5a9f9045f22eb4975ec5d6d0.
</commit_message>
<xml_diff>
--- a/tests/fixtures/formats/sample_headers.xlsx
+++ b/tests/fixtures/formats/sample_headers.xlsx
@@ -5,11 +5,10 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -147,11 +146,11 @@
   </sheetPr>
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -193,27 +192,4 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <sheetData/>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
 </file>
</xml_diff>